<commit_message>
cambio en la presentación
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Vale/ajuste/nuevo/regresiones_completo.xlsx
+++ b/Archivos de trabajo/Vale/ajuste/nuevo/regresiones_completo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcorvalan\Desktop\Trabajo\Paper-ITCRM.SF\Archivos de trabajo\Vale\ajuste\nuevo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF3F37C-3325-4FB3-8D18-0F5D42FF99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFAD576-2F53-40AE-B638-3225E5504AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -522,28 +522,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -666,27 +644,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -695,42 +720,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,860 +1018,861 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="21" customWidth="1"/>
-    <col min="5" max="7" width="18.140625" style="21" customWidth="1"/>
-    <col min="8" max="10" width="18.85546875" style="21" customWidth="1"/>
-    <col min="11" max="12" width="24.5703125" style="21" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="2.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
+    <col min="6" max="8" width="18.140625" style="14" customWidth="1"/>
+    <col min="9" max="11" width="18.85546875" style="14" customWidth="1"/>
+    <col min="12" max="13" width="24.5703125" style="14" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" style="14" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="20" t="s">
+    <row r="1" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="19"/>
+      <c r="C2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="2" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" s="16" t="s">
+      <c r="J4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="L4" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="M4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10">
+      <c r="H6" s="6"/>
+      <c r="I6" s="7">
         <v>-0.04</v>
       </c>
-      <c r="I6" s="11">
+      <c r="J6" s="8">
         <v>-8.5000000000000006E-2</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6"/>
+      <c r="L6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="12" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="12" t="s">
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7">
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G8" s="5">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="6">
         <v>-0.183</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="7" t="s">
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="7" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="K9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="13">
+      <c r="C10" s="10">
         <v>0.33400000000000002</v>
       </c>
-      <c r="C10" s="14">
+      <c r="D10" s="11">
         <v>0.30199999999999999</v>
       </c>
-      <c r="D10" s="15">
+      <c r="E10" s="12">
         <v>0.17599999999999999</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="10">
         <v>0.33200000000000002</v>
       </c>
-      <c r="F10" s="14">
+      <c r="G10" s="11">
         <v>0.29899999999999999</v>
       </c>
-      <c r="G10" s="15">
+      <c r="H10" s="12">
         <v>0.17699999999999999</v>
       </c>
-      <c r="H10" s="13">
+      <c r="I10" s="10">
         <v>0.82699999999999996</v>
       </c>
-      <c r="I10" s="14">
+      <c r="J10" s="11">
         <v>0.70799999999999996</v>
       </c>
-      <c r="J10" s="15">
+      <c r="K10" s="12">
         <v>0.71</v>
       </c>
-      <c r="K10" s="13">
+      <c r="L10" s="10">
         <v>0.82699999999999996</v>
       </c>
-      <c r="L10" s="14">
+      <c r="M10" s="11">
         <v>0.70699999999999996</v>
       </c>
-      <c r="M10" s="15">
+      <c r="N10" s="12">
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="20" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="2" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="3" t="s">
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="C13" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K13" s="16" t="s">
+      <c r="J13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="L13" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="M13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="K14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="N14" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="6"/>
+      <c r="L15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="M15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="12" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="12" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="12" t="s">
+      <c r="L16" s="4"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="7" t="s">
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="M17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="N17" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="7" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="K18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="M18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="M18" s="9" t="s">
+      <c r="N18" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="E19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="H19" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="I19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="J19" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="K19" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="L19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L19" s="14" t="s">
+      <c r="M19" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="N19" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="2" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="3" t="s">
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="C22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E22" s="16" t="s">
+      <c r="D22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="G22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K22" s="16" t="s">
+      <c r="J22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="L22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="M22" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="M22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="K23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="L23" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="M23" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="N23" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="J24" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="10" t="s">
+      <c r="K24" s="6"/>
+      <c r="L24" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="L24" s="11" t="s">
+      <c r="M24" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="12" t="s">
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="12" t="s">
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="12" t="s">
+      <c r="L25" s="4"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="7" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="G26" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="H26" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="7" t="s">
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="M26" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="M26" s="9" t="s">
+      <c r="N26" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="7" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="K27" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="L27" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="M27" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="M27" s="9" t="s">
+      <c r="N27" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="C28" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="E28" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="F28" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="G28" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="H28" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="I28" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="J28" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="K28" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="L28" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="M28" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="M28" s="15" t="s">
+      <c r="N28" s="12" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>